<commit_message>
Used shorter labels for strategy domains.
</commit_message>
<xml_diff>
--- a/assessments/srl/SRL-Items.xlsx
+++ b/assessments/srl/SRL-Items.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/DAACS-Deployment/assessments/srl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/Projects/DAACS-Github/DAACS-Website/assessments/srl/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -935,16 +935,16 @@
     <t>Mindset</t>
   </si>
   <si>
-    <t>Strategies for Managing Time</t>
-  </si>
-  <si>
-    <t>Strategies for Managing Environment</t>
-  </si>
-  <si>
-    <t>Strategies for Help Seeking</t>
-  </si>
-  <si>
-    <t>Strategies for Understanding</t>
+    <t>Managing Time</t>
+  </si>
+  <si>
+    <t>Help Seeking</t>
+  </si>
+  <si>
+    <t>Managing Environment</t>
+  </si>
+  <si>
+    <t>Understanding</t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1313,10 @@
   <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
+      <selection pane="bottomRight" activeCell="F64" sqref="A1:N121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1458,7 +1458,7 @@
         <v>294</v>
       </c>
       <c r="F5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>218</v>
@@ -1504,7 +1504,7 @@
         <v>294</v>
       </c>
       <c r="F7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>120</v>
@@ -2658,7 +2658,7 @@
         <v>294</v>
       </c>
       <c r="F62" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>202</v>
@@ -3273,7 +3273,7 @@
         <v>294</v>
       </c>
       <c r="F98" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>179</v>
@@ -3467,7 +3467,7 @@
         <v>294</v>
       </c>
       <c r="F111" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>88</v>
@@ -3608,7 +3608,7 @@
         <v>294</v>
       </c>
       <c r="F120" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>205</v>

</xml_diff>